<commit_message>
updated the last of the &, I hope!  Omar finally got back to me.
</commit_message>
<xml_diff>
--- a/documents/CRC and Diagram/CRC Cards.xlsx
+++ b/documents/CRC and Diagram/CRC Cards.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="303">
   <si>
     <t>Global</t>
   </si>
@@ -7832,146 +7832,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>) U (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">a2 &amp; !a3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp; P)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &amp; (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>!a3)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &amp; P)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> U a3))))</t>
-    </r>
-  </si>
-  <si>
-    <t>What I think</t>
-  </si>
-  <si>
-    <t>What Omar thinks</t>
-  </si>
-  <si>
-    <r>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">a1 &amp; !a2 &amp; !a3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&amp; P)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &amp; ((!a2 &amp; !a3)          U (</t>
     </r>
     <r>
       <rPr>
@@ -20946,19 +20806,11 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="44" t="s">
-        <v>305</v>
-      </c>
-      <c r="B31" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="44" t="s">
-        <v>302</v>
-      </c>
-      <c r="B32" t="s">
-        <v>303</v>
-      </c>
+      <c r="A32" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>